<commit_message>
looking good, got rid of life span
</commit_message>
<xml_diff>
--- a/FebInsectNutrition.xlsx
+++ b/FebInsectNutrition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive - University of Guelph\Documents\WEB lab\InsectNutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0466537-22E4-490D-A759-649FC153410B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620841E3-F89C-4326-9D6B-F21E9D76E442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="133">
   <si>
     <t>Month</t>
   </si>
@@ -435,9 +435,6 @@
     <t xml:space="preserve">Limnephilidae </t>
   </si>
   <si>
-    <t xml:space="preserve">August </t>
-  </si>
-  <si>
     <t>lasiocampidae</t>
   </si>
   <si>
@@ -469,6 +466,12 @@
   </si>
   <si>
     <t>Lipid_Amount</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>August</t>
   </si>
 </sst>
 </file>
@@ -709,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -748,21 +751,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -776,9 +776,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -821,6 +819,9 @@
       <fill>
         <patternFill patternType="none"/>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -902,35 +903,35 @@
     <tableColumn id="2" xr3:uid="{9119C412-CD23-4B3B-AF47-CAED021A465F}" name="Label " dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{E64482D3-C531-4E82-B5DC-2DE5A01129BA}" name="Order" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{95C735DD-8A4E-474F-BC7E-D08DD45CF357}" name="Family" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{23E6C9DC-3EC0-45AF-9190-11B074B0F848}" name="Sample_ID" dataDxfId="3">
+    <tableColumn id="13" xr3:uid="{23E6C9DC-3EC0-45AF-9190-11B074B0F848}" name="Sample_ID" dataDxfId="14">
       <calculatedColumnFormula>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{20134590-1C5C-4350-957D-9054D42CCB95}" name="Size" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{DF84E66E-4297-4E5E-A373-C719FF61958C}" name="Quantity" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{7B3296E8-7A8E-411A-B119-7837F8C7D940}" name="Envelope+Staple weight" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{D8573E08-DC5B-4B1E-950A-F1670263DE70}" name="Bugs+Envelope Weight" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{EF259457-1D66-478D-A4C7-E0A16F055B5C}" name="Insect_Weight" dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{20134590-1C5C-4350-957D-9054D42CCB95}" name="Size" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{DF84E66E-4297-4E5E-A373-C719FF61958C}" name="Quantity" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{7B3296E8-7A8E-411A-B119-7837F8C7D940}" name="Envelope+Staple weight" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{D8573E08-DC5B-4B1E-950A-F1670263DE70}" name="Bugs+Envelope Weight" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{EF259457-1D66-478D-A4C7-E0A16F055B5C}" name="Insect_Weight" dataDxfId="9">
       <calculatedColumnFormula>Table1[[#This Row],[Bugs+Envelope Weight]]-Table1[[#This Row],[Envelope+Staple weight]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{215B89B5-8EFF-44FC-9292-6932B21076A5}" name="avg bug size" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{215B89B5-8EFF-44FC-9292-6932B21076A5}" name="avg bug size" dataDxfId="8">
       <calculatedColumnFormula>Table1[[#This Row],[Insect_Weight]]/Table1[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{87A87AC7-8CDC-49ED-8517-9B50EA58D73F}" name="Dry Weight 1" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{8D712842-62A5-4FD8-A2C8-AED45499FE93}" name="Drying smaller?" dataDxfId="7">
+    <tableColumn id="11" xr3:uid="{87A87AC7-8CDC-49ED-8517-9B50EA58D73F}" name="Dry Weight 1" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{8D712842-62A5-4FD8-A2C8-AED45499FE93}" name="Drying smaller?" dataDxfId="6">
       <calculatedColumnFormula>L2&lt;I2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BC1C00DF-B5D1-486B-AEB1-081DDB25B98E}" name="Dry_Weight_Final" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{6154829C-15BC-4747-A80E-9C7788EAEEFE}" name="Dry_Weight" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{BC1C00DF-B5D1-486B-AEB1-081DDB25B98E}" name="Dry_Weight_Final" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{6154829C-15BC-4747-A80E-9C7788EAEEFE}" name="Dry_Weight" dataDxfId="4">
       <calculatedColumnFormula>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{ECFA0826-7ADF-4A03-978C-23FFE61FD57F}" name="Lipid Free Weight with envelope" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{EA7ECF17-5ECA-4F4F-BF33-ED98317D0FE4}" name="Lipid_Free_Weight" dataDxfId="1">
+    <tableColumn id="14" xr3:uid="{ECFA0826-7ADF-4A03-978C-23FFE61FD57F}" name="Lipid Free Weight with envelope" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{EA7ECF17-5ECA-4F4F-BF33-ED98317D0FE4}" name="Lipid_Free_Weight" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{FBADBBB3-BF0C-4AAD-A24C-03B0A2E49E2F}" name="Lipid_Amount" dataDxfId="0">
+    <tableColumn id="19" xr3:uid="{FBADBBB3-BF0C-4AAD-A24C-03B0A2E49E2F}" name="Lipid_Amount" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CBE151ED-7056-4EA6-B653-D13AE09FC373}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{CBE151ED-7056-4EA6-B653-D13AE09FC373}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1910,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7242F0B0-994C-45C6-A465-BA1D3A5A3292}">
   <dimension ref="A1:S154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1949,7 @@
         <v>86</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>87</v>
@@ -1963,7 +1964,7 @@
         <v>90</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K1" s="24" t="s">
         <v>91</v>
@@ -1978,16 +1979,16 @@
         <v>94</v>
       </c>
       <c r="O1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="R1" s="39" t="s">
         <v>130</v>
-      </c>
-      <c r="Q1" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="R1" s="40" t="s">
-        <v>131</v>
       </c>
       <c r="S1" t="s">
         <v>95</v>
@@ -2047,11 +2048,11 @@
       <c r="P2" s="10">
         <v>0.45029999999999998</v>
       </c>
-      <c r="Q2" s="38">
+      <c r="Q2" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.2299999999999986E-2</v>
       </c>
-      <c r="R2" s="38">
+      <c r="R2" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>8.5700000000000054E-2</v>
       </c>
@@ -2110,11 +2111,11 @@
       <c r="P3" s="10">
         <v>0.4516</v>
       </c>
-      <c r="Q3" s="38">
+      <c r="Q3" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.5600000000000012E-2</v>
       </c>
-      <c r="R3" s="38">
+      <c r="R3" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>7.8400000000000025E-2</v>
       </c>
@@ -2173,11 +2174,11 @@
       <c r="P4" s="10">
         <v>0.45469999999999999</v>
       </c>
-      <c r="Q4" s="38">
+      <c r="Q4" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.3699999999999999E-2</v>
       </c>
-      <c r="R4" s="38">
+      <c r="R4" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.10330000000000006</v>
       </c>
@@ -2234,11 +2235,11 @@
       <c r="P5" s="10">
         <v>0.45660000000000001</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.2600000000000018E-2</v>
       </c>
-      <c r="R5" s="38">
+      <c r="R5" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.13439999999999996</v>
       </c>
@@ -2256,7 +2257,7 @@
       <c r="D6" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="38" t="str">
+      <c r="E6" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Noctuidae&lt;1</v>
       </c>
@@ -2423,11 +2424,11 @@
       <c r="P8" s="34">
         <v>0.46129999999999999</v>
       </c>
-      <c r="Q8" s="41">
+      <c r="Q8">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.2299999999999995E-2</v>
       </c>
-      <c r="R8" s="41">
+      <c r="R8">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>8.1699999999999939E-2</v>
       </c>
@@ -2484,11 +2485,11 @@
       <c r="P9" s="10">
         <v>0.46560000000000001</v>
       </c>
-      <c r="Q9" s="38">
+      <c r="Q9" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.5600000000000021E-2</v>
       </c>
-      <c r="R9" s="38">
+      <c r="R9" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>7.4400000000000022E-2</v>
       </c>
@@ -2545,11 +2546,11 @@
       <c r="P10" s="10">
         <v>0.47060000000000002</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.2600000000000018E-2</v>
       </c>
-      <c r="R10" s="38">
+      <c r="R10" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.10439999999999994</v>
       </c>
@@ -2567,7 +2568,7 @@
       <c r="D11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="38" t="str">
+      <c r="E11" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Leptoceridae</v>
       </c>
@@ -2606,11 +2607,11 @@
       <c r="P11" s="10">
         <v>0.47520000000000001</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q11" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.6200000000000028E-2</v>
       </c>
-      <c r="R11" s="38">
+      <c r="R11" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.17580000000000001</v>
       </c>
@@ -2667,11 +2668,11 @@
       <c r="P12" s="34">
         <v>0.48099999999999998</v>
       </c>
-      <c r="Q12" s="41">
+      <c r="Q12">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>4.3999999999999984E-2</v>
       </c>
-      <c r="R12" s="41">
+      <c r="R12">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>8.1000000000000072E-2</v>
       </c>
@@ -2728,11 +2729,11 @@
       <c r="P13" s="10">
         <v>0.48139999999999999</v>
       </c>
-      <c r="Q13" s="38">
+      <c r="Q13" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>4.3399999999999994E-2</v>
       </c>
-      <c r="R13" s="38">
+      <c r="R13" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11759999999999998</v>
       </c>
@@ -2791,11 +2792,11 @@
       <c r="P14" s="10">
         <v>0.48149999999999998</v>
       </c>
-      <c r="Q14" s="38">
+      <c r="Q14" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.3499999999999992E-2</v>
       </c>
-      <c r="R14" s="38">
+      <c r="R14" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11649999999999999</v>
       </c>
@@ -2854,11 +2855,11 @@
       <c r="P15" s="10">
         <v>0.4899</v>
       </c>
-      <c r="Q15" s="38">
+      <c r="Q15" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.2899999999999985E-2</v>
       </c>
-      <c r="R15" s="38">
+      <c r="R15" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>9.4099999999999961E-2</v>
       </c>
@@ -2915,11 +2916,11 @@
       <c r="P16" s="10">
         <v>0.49080000000000001</v>
       </c>
-      <c r="Q16" s="38">
+      <c r="Q16" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.4800000000000024E-2</v>
       </c>
-      <c r="R16" s="38">
+      <c r="R16" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.22619999999999996</v>
       </c>
@@ -2937,7 +2938,7 @@
       <c r="D17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="39" t="str">
+      <c r="E17" s="38" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Microlep</v>
       </c>
@@ -2978,11 +2979,11 @@
       <c r="P17" s="10">
         <v>0.49130000000000001</v>
       </c>
-      <c r="Q17" s="38">
+      <c r="Q17" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>4.5300000000000007E-2</v>
       </c>
-      <c r="R17" s="38">
+      <c r="R17" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>6.5700000000000036E-2</v>
       </c>
@@ -3044,11 +3045,11 @@
       <c r="P18" s="10">
         <v>0.49790000000000001</v>
       </c>
-      <c r="Q18" s="38">
+      <c r="Q18" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.889999999999999E-2</v>
       </c>
-      <c r="R18" s="38">
+      <c r="R18" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>8.6099999999999954E-2</v>
       </c>
@@ -3107,11 +3108,11 @@
       <c r="P19" s="10">
         <v>0.50449999999999995</v>
       </c>
-      <c r="Q19" s="38">
+      <c r="Q19" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.0499999999999934E-2</v>
       </c>
-      <c r="R19" s="38">
+      <c r="R19" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11050000000000004</v>
       </c>
@@ -3173,11 +3174,11 @@
       <c r="P20" s="34">
         <v>0.50519999999999998</v>
       </c>
-      <c r="Q20" s="41">
+      <c r="Q20">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.9199999999999984E-2</v>
       </c>
-      <c r="R20" s="41">
+      <c r="R20">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11280000000000001</v>
       </c>
@@ -3234,11 +3235,11 @@
       <c r="P21" s="10">
         <v>0.51880000000000004</v>
       </c>
-      <c r="Q21" s="38">
+      <c r="Q21" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>8.6800000000000044E-2</v>
       </c>
-      <c r="R21" s="38">
+      <c r="R21" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>4.3200000000000016E-2</v>
       </c>
@@ -3295,11 +3296,11 @@
       <c r="P22" s="10">
         <v>0.52390000000000003</v>
       </c>
-      <c r="Q22" s="38">
+      <c r="Q22" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>9.2900000000000038E-2</v>
       </c>
-      <c r="R22" s="38">
+      <c r="R22" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.30109999999999992</v>
       </c>
@@ -3361,11 +3362,11 @@
       <c r="P23" s="10">
         <v>0.52869999999999995</v>
       </c>
-      <c r="Q23" s="38">
+      <c r="Q23" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.10069999999999996</v>
       </c>
-      <c r="R23" s="38">
+      <c r="R23" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.23630000000000007</v>
       </c>
@@ -3424,11 +3425,11 @@
       <c r="P24" s="10">
         <v>0.53410000000000002</v>
       </c>
-      <c r="Q24" s="38">
+      <c r="Q24" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.10610000000000003</v>
       </c>
-      <c r="R24" s="38">
+      <c r="R24" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.24690000000000001</v>
       </c>
@@ -3446,7 +3447,7 @@
       <c r="D25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="39" t="str">
+      <c r="E25" s="38" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Hydroptilidae</v>
       </c>
@@ -3485,11 +3486,11 @@
       <c r="P25" s="10">
         <v>0.54310000000000003</v>
       </c>
-      <c r="Q25" s="38">
+      <c r="Q25" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>8.9100000000000013E-2</v>
       </c>
-      <c r="R25" s="38">
+      <c r="R25" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.10289999999999999</v>
       </c>
@@ -3548,11 +3549,11 @@
       <c r="P26" s="10">
         <v>0.55489999999999995</v>
       </c>
-      <c r="Q26" s="38">
+      <c r="Q26" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.11989999999999995</v>
       </c>
-      <c r="R26" s="38">
+      <c r="R26" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.28810000000000002</v>
       </c>
@@ -3609,11 +3610,11 @@
       <c r="P27" s="10">
         <v>0.60440000000000005</v>
       </c>
-      <c r="Q27" s="38">
+      <c r="Q27" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.18240000000000006</v>
       </c>
-      <c r="R27" s="38">
+      <c r="R27" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.38159999999999999</v>
       </c>
@@ -3670,11 +3671,11 @@
       <c r="P28" s="10">
         <v>0.64580000000000004</v>
       </c>
-      <c r="Q28" s="38">
+      <c r="Q28" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>8.80000000000003E-3</v>
       </c>
-      <c r="R28" s="38">
+      <c r="R28" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>9.319999999999995E-2</v>
       </c>
@@ -3733,11 +3734,11 @@
       <c r="P29" s="10">
         <v>0.68240000000000001</v>
       </c>
-      <c r="Q29" s="38">
+      <c r="Q29" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.1399999999999966E-2</v>
       </c>
-      <c r="R29" s="38">
+      <c r="R29" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.10260000000000002</v>
       </c>
@@ -3796,11 +3797,11 @@
       <c r="P30" s="10">
         <v>0.68779999999999997</v>
       </c>
-      <c r="Q30" s="38">
+      <c r="Q30" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.7799999999999936E-2</v>
       </c>
-      <c r="R30" s="38">
+      <c r="R30" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.12519999999999998</v>
       </c>
@@ -3862,11 +3863,11 @@
       <c r="P31" s="10">
         <v>0.69130000000000003</v>
       </c>
-      <c r="Q31" s="38">
+      <c r="Q31" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.0299999999999985E-2</v>
       </c>
-      <c r="R31" s="38">
+      <c r="R31" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11770000000000003</v>
       </c>
@@ -3923,11 +3924,11 @@
       <c r="P32" s="10">
         <v>0.69699999999999995</v>
       </c>
-      <c r="Q32" s="38">
+      <c r="Q32" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.7999999999999914E-2</v>
       </c>
-      <c r="R32" s="38">
+      <c r="R32" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.15900000000000003</v>
       </c>
@@ -3986,11 +3987,11 @@
       <c r="P33" s="10">
         <v>0.69879999999999998</v>
       </c>
-      <c r="Q33" s="38">
+      <c r="Q33" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.8799999999999928E-2</v>
       </c>
-      <c r="R33" s="38">
+      <c r="R33" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11120000000000008</v>
       </c>
@@ -4049,11 +4050,11 @@
       <c r="P34" s="10">
         <v>0.70730000000000004</v>
       </c>
-      <c r="Q34" s="38">
+      <c r="Q34" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.2299999999999995E-2</v>
       </c>
-      <c r="R34" s="38">
+      <c r="R34" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11370000000000002</v>
       </c>
@@ -4074,7 +4075,7 @@
       <c r="D35" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="39" t="str">
+      <c r="E35" s="38" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Elateridae</v>
       </c>
@@ -4114,11 +4115,11 @@
       <c r="P35" s="10">
         <v>0.70760000000000001</v>
       </c>
-      <c r="Q35" s="38">
+      <c r="Q35" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.28160000000000002</v>
       </c>
-      <c r="R35" s="38">
+      <c r="R35" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.48140000000000011</v>
       </c>
@@ -4139,7 +4140,7 @@
       <c r="D36" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E36" s="38" t="str">
+      <c r="E36" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Brachycera</v>
       </c>
@@ -4178,11 +4179,11 @@
       <c r="P36" s="10">
         <v>0.70860000000000001</v>
       </c>
-      <c r="Q36" s="38">
+      <c r="Q36" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>4.159999999999997E-2</v>
       </c>
-      <c r="R36" s="38">
+      <c r="R36" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.14639999999999997</v>
       </c>
@@ -4200,7 +4201,7 @@
       <c r="D37" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E37" s="39" t="str">
+      <c r="E37" s="38" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Carabidae&gt;1</v>
       </c>
@@ -4241,11 +4242,11 @@
       <c r="P37" s="10">
         <v>0.71879999999999999</v>
       </c>
-      <c r="Q37" s="38">
+      <c r="Q37" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.2799999999999967E-2</v>
       </c>
-      <c r="R37" s="38">
+      <c r="R37" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.18620000000000003</v>
       </c>
@@ -4263,7 +4264,7 @@
       <c r="D38" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="39" t="str">
+      <c r="E38" s="38" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v xml:space="preserve">Nematocera </v>
       </c>
@@ -4302,11 +4303,11 @@
       <c r="P38" s="10">
         <v>0.71889999999999998</v>
       </c>
-      <c r="Q38" s="38">
+      <c r="Q38" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.1899999999999955E-2</v>
       </c>
-      <c r="R38" s="38">
+      <c r="R38" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>8.9100000000000068E-2</v>
       </c>
@@ -4324,7 +4325,7 @@
       <c r="D39" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E39" s="38" t="str">
+      <c r="E39" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Heteroceridae</v>
       </c>
@@ -4365,11 +4366,11 @@
       <c r="P39" s="10">
         <v>0.7198</v>
       </c>
-      <c r="Q39" s="38">
+      <c r="Q39" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.7799999999999945E-2</v>
       </c>
-      <c r="R39" s="38">
+      <c r="R39" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>9.5199999999999951E-2</v>
       </c>
@@ -4390,7 +4391,7 @@
       <c r="D40" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="39" t="str">
+      <c r="E40" s="38" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Staphylinidae</v>
       </c>
@@ -4429,11 +4430,11 @@
       <c r="P40" s="10">
         <v>0.72230000000000005</v>
       </c>
-      <c r="Q40" s="38">
+      <c r="Q40" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.7300000000000018E-2</v>
       </c>
-      <c r="R40" s="38">
+      <c r="R40" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11969999999999992</v>
       </c>
@@ -4492,11 +4493,11 @@
       <c r="P41" s="10">
         <v>0.73360000000000003</v>
       </c>
-      <c r="Q41" s="38">
+      <c r="Q41" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.8599999999999994E-2</v>
       </c>
-      <c r="R41" s="38">
+      <c r="R41" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>6.5400000000000014E-2</v>
       </c>
@@ -4580,7 +4581,7 @@
       <c r="D43" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="38" t="str">
+      <c r="E43" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Crambidae&gt;1</v>
       </c>
@@ -4684,11 +4685,11 @@
       <c r="P44" s="10">
         <v>0.73819999999999997</v>
       </c>
-      <c r="Q44" s="38">
+      <c r="Q44" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.29819999999999997</v>
       </c>
-      <c r="R44" s="38">
+      <c r="R44" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.45980000000000004</v>
       </c>
@@ -4747,11 +4748,11 @@
       <c r="P45" s="10">
         <v>0.74170000000000003</v>
       </c>
-      <c r="Q45" s="38">
+      <c r="Q45" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>7.2699999999999987E-2</v>
       </c>
-      <c r="R45" s="38">
+      <c r="R45" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.20629999999999993</v>
       </c>
@@ -4810,11 +4811,11 @@
       <c r="P46" s="10">
         <v>0.74570000000000003</v>
       </c>
-      <c r="Q46" s="38">
+      <c r="Q46" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>9.1700000000000004E-2</v>
       </c>
-      <c r="R46" s="38">
+      <c r="R46" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.25829999999999997</v>
       </c>
@@ -4873,11 +4874,11 @@
       <c r="P47" s="10">
         <v>0.74780000000000002</v>
       </c>
-      <c r="Q47" s="38">
+      <c r="Q47" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>8.9799999999999991E-2</v>
       </c>
-      <c r="R47" s="38">
+      <c r="R47" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.17420000000000002</v>
       </c>
@@ -4934,11 +4935,11 @@
       <c r="P48" s="10">
         <v>0.75460000000000005</v>
       </c>
-      <c r="Q48" s="38">
+      <c r="Q48" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>9.9600000000000022E-2</v>
       </c>
-      <c r="R48" s="38">
+      <c r="R48" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.1913999999999999</v>
       </c>
@@ -4995,11 +4996,11 @@
       <c r="P49" s="10">
         <v>0.78210000000000002</v>
       </c>
-      <c r="Q49" s="38">
+      <c r="Q49" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.12309999999999999</v>
       </c>
-      <c r="R49" s="38">
+      <c r="R49" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.18589999999999995</v>
       </c>
@@ -5056,11 +5057,11 @@
       <c r="P50" s="10">
         <v>0.78959999999999997</v>
       </c>
-      <c r="Q50" s="38">
+      <c r="Q50" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.12859999999999994</v>
       </c>
-      <c r="R50" s="38">
+      <c r="R50" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.27539999999999998</v>
       </c>
@@ -5119,11 +5120,11 @@
       <c r="P51" s="10">
         <v>0.79659999999999997</v>
       </c>
-      <c r="Q51" s="38">
+      <c r="Q51" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.14359999999999995</v>
       </c>
-      <c r="R51" s="38">
+      <c r="R51" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.30140000000000011</v>
       </c>
@@ -5180,11 +5181,11 @@
       <c r="P52" s="10">
         <v>0.79790000000000005</v>
       </c>
-      <c r="Q52" s="38">
+      <c r="Q52" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.12690000000000001</v>
       </c>
-      <c r="R52" s="38">
+      <c r="R52" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.38109999999999999</v>
       </c>
@@ -5243,11 +5244,11 @@
       <c r="P53" s="10">
         <v>0.84960000000000002</v>
       </c>
-      <c r="Q53" s="38">
+      <c r="Q53" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.18859999999999999</v>
       </c>
-      <c r="R53" s="38">
+      <c r="R53" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.47339999999999993</v>
       </c>
@@ -5306,11 +5307,11 @@
       <c r="P54" s="10">
         <v>0.85709999999999997</v>
       </c>
-      <c r="Q54" s="38">
+      <c r="Q54" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.19209999999999994</v>
       </c>
-      <c r="R54" s="38">
+      <c r="R54" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.46989999999999998</v>
       </c>
@@ -5369,11 +5370,11 @@
       <c r="P55" s="10">
         <v>0.86150000000000004</v>
       </c>
-      <c r="Q55" s="38">
+      <c r="Q55" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.20250000000000001</v>
       </c>
-      <c r="R55" s="38">
+      <c r="R55" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.50250000000000006</v>
       </c>
@@ -5430,11 +5431,11 @@
       <c r="P56" s="10">
         <v>0.87590000000000001</v>
       </c>
-      <c r="Q56" s="38">
+      <c r="Q56" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.44390000000000002</v>
       </c>
-      <c r="R56" s="38">
+      <c r="R56" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.79710000000000014</v>
       </c>
@@ -5493,11 +5494,11 @@
       <c r="P57" s="10">
         <v>0.88180000000000003</v>
       </c>
-      <c r="Q57" s="38">
+      <c r="Q57" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.2218</v>
       </c>
-      <c r="R57" s="38">
+      <c r="R57" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.69420000000000004</v>
       </c>
@@ -5554,11 +5555,11 @@
       <c r="P58" s="10">
         <v>0.9274</v>
       </c>
-      <c r="Q58" s="38">
+      <c r="Q58" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.25539999999999996</v>
       </c>
-      <c r="R58" s="38">
+      <c r="R58" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.81759999999999999</v>
       </c>
@@ -5615,11 +5616,11 @@
       <c r="P59" s="10">
         <v>0.93289999999999995</v>
       </c>
-      <c r="Q59" s="38">
+      <c r="Q59" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.25789999999999991</v>
       </c>
-      <c r="R59" s="38">
+      <c r="R59" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.55710000000000004</v>
       </c>
@@ -5676,11 +5677,11 @@
       <c r="P60" s="10">
         <v>0.96120000000000005</v>
       </c>
-      <c r="Q60" s="38">
+      <c r="Q60" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.29920000000000002</v>
       </c>
-      <c r="R60" s="38">
+      <c r="R60" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.53580000000000005</v>
       </c>
@@ -5739,11 +5740,11 @@
       <c r="P61" s="10">
         <v>0.96940000000000004</v>
       </c>
-      <c r="Q61" s="38">
+      <c r="Q61" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.30940000000000001</v>
       </c>
-      <c r="R61" s="38">
+      <c r="R61" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.61559999999999993</v>
       </c>
@@ -5800,11 +5801,11 @@
       <c r="P62" s="10">
         <v>0.98540000000000005</v>
       </c>
-      <c r="Q62" s="38">
+      <c r="Q62" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.31740000000000002</v>
       </c>
-      <c r="R62" s="38">
+      <c r="R62" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.85860000000000014</v>
       </c>
@@ -5863,11 +5864,11 @@
       <c r="P63" s="10">
         <v>0.99119999999999997</v>
       </c>
-      <c r="Q63" s="38">
+      <c r="Q63" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.32919999999999994</v>
       </c>
-      <c r="R63" s="38">
+      <c r="R63" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.50280000000000002</v>
       </c>
@@ -5885,7 +5886,7 @@
       <c r="D64" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E64" s="38" t="str">
+      <c r="E64" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Geometridae&gt;1</v>
       </c>
@@ -5926,11 +5927,11 @@
       <c r="P64" s="10">
         <v>1.0178</v>
       </c>
-      <c r="Q64" s="38">
+      <c r="Q64" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.35780000000000001</v>
       </c>
-      <c r="R64" s="38">
+      <c r="R64" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.6801999999999998</v>
       </c>
@@ -5989,11 +5990,11 @@
       <c r="P65" s="10">
         <v>1.0561</v>
       </c>
-      <c r="Q65" s="38">
+      <c r="Q65" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.3931</v>
       </c>
-      <c r="R65" s="38">
+      <c r="R65" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.59989999999999988</v>
       </c>
@@ -6052,11 +6053,11 @@
       <c r="P66" s="10">
         <v>1.0984</v>
       </c>
-      <c r="Q66" s="38">
+      <c r="Q66" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.44640000000000002</v>
       </c>
-      <c r="R66" s="38">
+      <c r="R66" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.98659999999999981</v>
       </c>
@@ -6113,11 +6114,11 @@
       <c r="P67" s="10">
         <v>1.1153999999999999</v>
       </c>
-      <c r="Q67" s="38">
+      <c r="Q67" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.46539999999999992</v>
       </c>
-      <c r="R67" s="38">
+      <c r="R67" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.77859999999999985</v>
       </c>
@@ -6174,11 +6175,11 @@
       <c r="P68" s="10">
         <v>1.1194999999999999</v>
       </c>
-      <c r="Q68" s="38">
+      <c r="Q68" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.46249999999999991</v>
       </c>
-      <c r="R68" s="38">
+      <c r="R68" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.97150000000000025</v>
       </c>
@@ -6237,11 +6238,11 @@
       <c r="P69" s="10">
         <v>1.1301000000000001</v>
       </c>
-      <c r="Q69" s="38">
+      <c r="Q69" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.47210000000000008</v>
       </c>
-      <c r="R69" s="38">
+      <c r="R69" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.0789</v>
       </c>
@@ -6298,11 +6299,11 @@
       <c r="P70" s="10">
         <v>1.1521999999999999</v>
       </c>
-      <c r="Q70" s="38">
+      <c r="Q70" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.49519999999999986</v>
       </c>
-      <c r="R70" s="38">
+      <c r="R70" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.2838000000000001</v>
       </c>
@@ -6361,11 +6362,11 @@
       <c r="P71" s="10">
         <v>1.1776</v>
       </c>
-      <c r="Q71" s="38">
+      <c r="Q71" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.52059999999999995</v>
       </c>
-      <c r="R71" s="38">
+      <c r="R71" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.0624000000000002</v>
       </c>
@@ -6424,11 +6425,11 @@
       <c r="P72" s="10">
         <v>1.2116</v>
       </c>
-      <c r="Q72" s="38">
+      <c r="Q72" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.55359999999999998</v>
       </c>
-      <c r="R72" s="38">
+      <c r="R72" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.4714</v>
       </c>
@@ -6487,11 +6488,11 @@
       <c r="P73" s="10">
         <v>1.266</v>
       </c>
-      <c r="Q73" s="38">
+      <c r="Q73" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.60199999999999998</v>
       </c>
-      <c r="R73" s="38">
+      <c r="R73" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.2599999999999998</v>
       </c>
@@ -6550,11 +6551,11 @@
       <c r="P74" s="10">
         <v>1.3057000000000001</v>
       </c>
-      <c r="Q74" s="38">
+      <c r="Q74" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.63770000000000004</v>
       </c>
-      <c r="R74" s="38">
+      <c r="R74" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.5452999999999997</v>
       </c>
@@ -6613,11 +6614,11 @@
       <c r="P75" s="10">
         <v>1.3057000000000001</v>
       </c>
-      <c r="Q75" s="38">
+      <c r="Q75" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.65770000000000006</v>
       </c>
-      <c r="R75" s="38">
+      <c r="R75" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.6152999999999995</v>
       </c>
@@ -6674,11 +6675,11 @@
       <c r="P76" s="10">
         <v>1.3371</v>
       </c>
-      <c r="Q76" s="38">
+      <c r="Q76" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.66809999999999992</v>
       </c>
-      <c r="R76" s="38">
+      <c r="R76" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.1189</v>
       </c>
@@ -6730,18 +6731,18 @@
       <c r="N77" s="8">
         <v>1.4219999999999999</v>
       </c>
-      <c r="O77" s="38">
+      <c r="O77" s="9">
         <f>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.7589999999999999</v>
       </c>
       <c r="P77" s="36">
         <v>1.3129999999999999</v>
       </c>
-      <c r="Q77" s="42">
+      <c r="Q77" s="40">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.64999999999999991</v>
       </c>
-      <c r="R77" s="42">
+      <c r="R77" s="40">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.3539999999999996</v>
       </c>
@@ -6798,11 +6799,11 @@
       <c r="P78" s="10">
         <v>0.754</v>
       </c>
-      <c r="Q78" s="38">
+      <c r="Q78" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>9.2999999999999972E-2</v>
       </c>
-      <c r="R78" s="38">
+      <c r="R78" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.15400000000000003</v>
       </c>
@@ -6820,7 +6821,7 @@
       <c r="D79" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E79" s="38" t="str">
+      <c r="E79" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Leptoceridae</v>
       </c>
@@ -6859,11 +6860,11 @@
       <c r="P79" s="10">
         <v>0.78</v>
       </c>
-      <c r="Q79" s="38">
+      <c r="Q79" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.11299999999999999</v>
       </c>
-      <c r="R79" s="38">
+      <c r="R79" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.16299999999999992</v>
       </c>
@@ -6922,11 +6923,11 @@
       <c r="P80" s="10">
         <v>0.79200000000000004</v>
       </c>
-      <c r="Q80" s="38">
+      <c r="Q80" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.13800000000000001</v>
       </c>
-      <c r="R80" s="38">
+      <c r="R80" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.19699999999999995</v>
       </c>
@@ -6944,7 +6945,7 @@
       <c r="D81" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E81" s="38" t="str">
+      <c r="E81" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Erebidae&lt;1</v>
       </c>
@@ -6985,11 +6986,11 @@
       <c r="P81" s="10">
         <v>0.67300000000000004</v>
       </c>
-      <c r="Q81" s="38">
+      <c r="Q81" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.5000000000000013E-2</v>
       </c>
-      <c r="R81" s="38">
+      <c r="R81" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>8.8999999999999968E-2</v>
       </c>
@@ -7048,11 +7049,11 @@
       <c r="P82" s="10">
         <v>0.879</v>
       </c>
-      <c r="Q82" s="38">
+      <c r="Q82" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="R82" s="38">
+      <c r="R82" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.46199999999999997</v>
       </c>
@@ -7070,7 +7071,7 @@
       <c r="D83" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E83" s="38" t="str">
+      <c r="E83" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Leptoceridae</v>
       </c>
@@ -7109,11 +7110,11 @@
       <c r="P83" s="10">
         <v>0.73</v>
       </c>
-      <c r="Q83" s="38">
+      <c r="Q83" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.1999999999999935E-2</v>
       </c>
-      <c r="R83" s="38">
+      <c r="R83" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.122</v>
       </c>
@@ -7131,7 +7132,7 @@
       <c r="D84" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E84" s="38" t="str">
+      <c r="E84" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Phryganeidae</v>
       </c>
@@ -7163,18 +7164,18 @@
       <c r="N84" s="8">
         <v>0.90400000000000003</v>
       </c>
-      <c r="O84" s="38">
+      <c r="O84" s="9">
         <f>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.23499999999999999</v>
       </c>
       <c r="P84" s="35">
         <v>0.86599999999999999</v>
       </c>
-      <c r="Q84" s="41">
+      <c r="Q84">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.19699999999999995</v>
       </c>
-      <c r="R84" s="41">
+      <c r="R84">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.43899999999999995</v>
       </c>
@@ -7233,11 +7234,11 @@
       <c r="P85" s="10">
         <v>0.79</v>
       </c>
-      <c r="Q85" s="38">
+      <c r="Q85" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.122</v>
       </c>
-      <c r="R85" s="38">
+      <c r="R85" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.26200000000000001</v>
       </c>
@@ -7296,11 +7297,11 @@
       <c r="P86" s="10">
         <v>0.72799999999999998</v>
       </c>
-      <c r="Q86" s="38">
+      <c r="Q86" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.799999999999994E-2</v>
       </c>
-      <c r="R86" s="38">
+      <c r="R86" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.16100000000000003</v>
       </c>
@@ -7357,11 +7358,11 @@
       <c r="P87" s="10">
         <v>0.74299999999999999</v>
       </c>
-      <c r="Q87" s="38">
+      <c r="Q87" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>8.4999999999999964E-2</v>
       </c>
-      <c r="R87" s="38">
+      <c r="R87" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>7.0999999999999952E-2</v>
       </c>
@@ -7420,11 +7421,11 @@
       <c r="P88" s="10">
         <v>1.0629999999999999</v>
       </c>
-      <c r="Q88" s="38">
+      <c r="Q88" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.3919999999999999</v>
       </c>
-      <c r="R88" s="38">
+      <c r="R88" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.91100000000000003</v>
       </c>
@@ -7481,11 +7482,11 @@
       <c r="P89" s="10">
         <v>0.67900000000000005</v>
       </c>
-      <c r="Q89" s="38">
+      <c r="Q89" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.7000000000000015E-2</v>
       </c>
-      <c r="R89" s="38">
+      <c r="R89" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>9.5999999999999974E-2</v>
       </c>
@@ -7544,11 +7545,11 @@
       <c r="P90" s="10">
         <v>0.83599999999999997</v>
       </c>
-      <c r="Q90" s="38">
+      <c r="Q90" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.16299999999999992</v>
       </c>
-      <c r="R90" s="38">
+      <c r="R90" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.34700000000000009</v>
       </c>
@@ -7607,11 +7608,11 @@
       <c r="P91" s="10">
         <v>0.71699999999999997</v>
       </c>
-      <c r="Q91" s="38">
+      <c r="Q91" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.699999999999994E-2</v>
       </c>
-      <c r="R91" s="38">
+      <c r="R91" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.19000000000000006</v>
       </c>
@@ -7668,11 +7669,11 @@
       <c r="P92" s="10">
         <v>0.70099999999999996</v>
       </c>
-      <c r="Q92" s="38">
+      <c r="Q92" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.1999999999999917E-2</v>
       </c>
-      <c r="R92" s="38">
+      <c r="R92" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>7.1000000000000063E-2</v>
       </c>
@@ -7729,11 +7730,11 @@
       <c r="P93" s="10">
         <v>0.80700000000000005</v>
       </c>
-      <c r="Q93" s="38">
+      <c r="Q93" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.15300000000000002</v>
       </c>
-      <c r="R93" s="38">
+      <c r="R93" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.45399999999999985</v>
       </c>
@@ -7790,11 +7791,11 @@
       <c r="P94" s="10">
         <v>0.746</v>
       </c>
-      <c r="Q94" s="38">
+      <c r="Q94" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>7.8999999999999959E-2</v>
       </c>
-      <c r="R94" s="38">
+      <c r="R94" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.20999999999999996</v>
       </c>
@@ -7851,11 +7852,11 @@
       <c r="P95" s="10">
         <v>0.94599999999999995</v>
       </c>
-      <c r="Q95" s="38">
+      <c r="Q95" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.27499999999999991</v>
       </c>
-      <c r="R95" s="38">
+      <c r="R95" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.68900000000000006</v>
       </c>
@@ -7907,18 +7908,18 @@
       <c r="N96" s="8">
         <v>0.69</v>
       </c>
-      <c r="O96" s="38">
+      <c r="O96" s="9">
         <f>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.7999999999999914E-2</v>
       </c>
       <c r="P96" s="35">
         <v>0.67800000000000005</v>
       </c>
-      <c r="Q96" s="41">
+      <c r="Q96">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.6000000000000014E-2</v>
       </c>
-      <c r="R96" s="41">
+      <c r="R96">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.121</v>
       </c>
@@ -7975,11 +7976,11 @@
       <c r="P97" s="10">
         <v>1.04</v>
       </c>
-      <c r="Q97" s="38">
+      <c r="Q97" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.378</v>
       </c>
-      <c r="R97" s="38">
+      <c r="R97" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.0670000000000002</v>
       </c>
@@ -8031,18 +8032,18 @@
       <c r="N98" s="8">
         <v>0.47199999999999998</v>
       </c>
-      <c r="O98" s="38">
+      <c r="O98" s="9">
         <f>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.1999999999999973E-2</v>
       </c>
       <c r="P98" s="35">
         <v>0.46200000000000002</v>
       </c>
-      <c r="Q98" s="41">
+      <c r="Q98">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.200000000000002E-2</v>
       </c>
-      <c r="R98" s="41">
+      <c r="R98">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>9.7000000000000031E-2</v>
       </c>
@@ -8099,11 +8100,11 @@
       <c r="P99" s="10">
         <v>0.76500000000000001</v>
       </c>
-      <c r="Q99" s="38">
+      <c r="Q99" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.700000000000006E-2</v>
       </c>
-      <c r="R99" s="38">
+      <c r="R99" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.19999999999999996</v>
       </c>
@@ -8160,11 +8161,11 @@
       <c r="P100" s="10">
         <v>0.997</v>
       </c>
-      <c r="Q100" s="38">
+      <c r="Q100" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.32899999999999996</v>
       </c>
-      <c r="R100" s="38">
+      <c r="R100" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.24099999999999999</v>
       </c>
@@ -8182,7 +8183,7 @@
       <c r="D101" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E101" s="38" t="str">
+      <c r="E101" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Notodontidae</v>
       </c>
@@ -8221,11 +8222,11 @@
       <c r="P101" s="10">
         <v>0.95</v>
       </c>
-      <c r="Q101" s="38">
+      <c r="Q101" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.28299999999999992</v>
       </c>
-      <c r="R101" s="38">
+      <c r="R101" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.82899999999999996</v>
       </c>
@@ -8284,11 +8285,11 @@
       <c r="P102" s="10">
         <v>0.81</v>
       </c>
-      <c r="Q102" s="38">
+      <c r="Q102" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="R102" s="38">
+      <c r="R102" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.31699999999999995</v>
       </c>
@@ -8306,7 +8307,7 @@
       <c r="D103" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E103" s="38" t="str">
+      <c r="E103" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Crambidae&lt;1</v>
       </c>
@@ -8347,11 +8348,11 @@
       <c r="P103" s="10">
         <v>0.747</v>
       </c>
-      <c r="Q103" s="38">
+      <c r="Q103" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>7.999999999999996E-2</v>
       </c>
-      <c r="R103" s="38">
+      <c r="R103" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.2619999999999999</v>
       </c>
@@ -8410,11 +8411,11 @@
       <c r="P104" s="10">
         <v>0.69899999999999995</v>
       </c>
-      <c r="Q104" s="38">
+      <c r="Q104" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.2999999999999918E-2</v>
       </c>
-      <c r="R104" s="38">
+      <c r="R104" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.14900000000000002</v>
       </c>
@@ -8471,11 +8472,11 @@
       <c r="P105" s="10">
         <v>0.99099999999999999</v>
       </c>
-      <c r="Q105" s="38">
+      <c r="Q105" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.31599999999999995</v>
       </c>
-      <c r="R105" s="38">
+      <c r="R105" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.85500000000000009</v>
       </c>
@@ -8534,11 +8535,11 @@
       <c r="P106" s="10">
         <v>0.81599999999999995</v>
       </c>
-      <c r="Q106" s="38">
+      <c r="Q106" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.14399999999999991</v>
       </c>
-      <c r="R106" s="38">
+      <c r="R106" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.35500000000000009</v>
       </c>
@@ -8595,11 +8596,11 @@
       <c r="P107" s="10">
         <v>1.5629999999999999</v>
       </c>
-      <c r="Q107" s="38">
+      <c r="Q107" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.8919999999999999</v>
       </c>
-      <c r="R107" s="38">
+      <c r="R107" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.4</v>
       </c>
@@ -8658,11 +8659,11 @@
       <c r="P108" s="10">
         <v>0.94299999999999995</v>
       </c>
-      <c r="Q108" s="38">
+      <c r="Q108" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.28299999999999992</v>
       </c>
-      <c r="R108" s="38">
+      <c r="R108" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.61</v>
       </c>
@@ -8719,11 +8720,11 @@
       <c r="P109" s="10">
         <v>1.181</v>
       </c>
-      <c r="Q109" s="38">
+      <c r="Q109" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.52500000000000002</v>
       </c>
-      <c r="R109" s="38">
+      <c r="R109" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.98399999999999987</v>
       </c>
@@ -8782,11 +8783,11 @@
       <c r="P110" s="10">
         <v>0.68200000000000005</v>
       </c>
-      <c r="Q110" s="38">
+      <c r="Q110" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.24700000000000005</v>
       </c>
-      <c r="R110" s="38">
+      <c r="R110" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.3409999999999998</v>
       </c>
@@ -8845,11 +8846,11 @@
       <c r="P111" s="10">
         <v>0.50800000000000001</v>
       </c>
-      <c r="Q111" s="38">
+      <c r="Q111" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.2E-2</v>
       </c>
-      <c r="R111" s="38">
+      <c r="R111" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.14300000000000002</v>
       </c>
@@ -8908,11 +8909,11 @@
       <c r="P112" s="10">
         <v>0.871</v>
       </c>
-      <c r="Q112" s="38">
+      <c r="Q112" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.20299999999999996</v>
       </c>
-      <c r="R112" s="38">
+      <c r="R112" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.39399999999999991</v>
       </c>
@@ -8969,11 +8970,11 @@
       <c r="P113" s="10">
         <v>1.2330000000000001</v>
       </c>
-      <c r="Q113" s="38">
+      <c r="Q113" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.55100000000000005</v>
       </c>
-      <c r="R113" s="38">
+      <c r="R113" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.016</v>
       </c>
@@ -8991,7 +8992,7 @@
       <c r="D114" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E114" s="38" t="str">
+      <c r="E114" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Crambidae&gt;1</v>
       </c>
@@ -9032,11 +9033,11 @@
       <c r="P114" s="10">
         <v>0.78200000000000003</v>
       </c>
-      <c r="Q114" s="38">
+      <c r="Q114" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.11599999999999999</v>
       </c>
-      <c r="R114" s="38">
+      <c r="R114" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.28299999999999992</v>
       </c>
@@ -9093,11 +9094,11 @@
       <c r="P115" s="10">
         <v>0.51300000000000001</v>
       </c>
-      <c r="Q115" s="38">
+      <c r="Q115" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.7999999999999996E-2</v>
       </c>
-      <c r="R115" s="38">
+      <c r="R115" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>9.2999999999999972E-2</v>
       </c>
@@ -9115,7 +9116,7 @@
       <c r="D116" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E116" s="38" t="str">
+      <c r="E116" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Erebidae&gt;1</v>
       </c>
@@ -9149,18 +9150,18 @@
       <c r="N116" s="8">
         <v>1.5660000000000001</v>
       </c>
-      <c r="O116" s="38">
+      <c r="O116" s="9">
         <f>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.89200000000000002</v>
       </c>
       <c r="P116" s="36">
         <v>1.4059999999999999</v>
       </c>
-      <c r="Q116" s="42">
+      <c r="Q116" s="40">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.73199999999999987</v>
       </c>
-      <c r="R116" s="42">
+      <c r="R116" s="40">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.6510000000000002</v>
       </c>
@@ -9217,11 +9218,11 @@
       <c r="P117" s="10">
         <v>0.47299999999999998</v>
       </c>
-      <c r="Q117" s="38">
+      <c r="Q117" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.9999999999999971E-2</v>
       </c>
-      <c r="R117" s="38">
+      <c r="R117" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.124</v>
       </c>
@@ -9239,7 +9240,7 @@
       <c r="D118" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E118" s="38" t="str">
+      <c r="E118" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>Carabidae&gt;1</v>
       </c>
@@ -9282,21 +9283,21 @@
         <f>0.7188/4*3</f>
         <v>0.53910000000000002</v>
       </c>
-      <c r="Q118" s="38">
+      <c r="Q118" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>-0.1169</v>
       </c>
-      <c r="R118" s="38">
+      <c r="R118" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.40790000000000004</v>
       </c>
       <c r="S118" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B119" s="7">
         <v>45883</v>
@@ -9348,18 +9349,18 @@
       <c r="P119" s="10">
         <v>1.046</v>
       </c>
-      <c r="Q119" s="38">
+      <c r="Q119" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.36499999999999999</v>
       </c>
-      <c r="R119" s="38">
+      <c r="R119" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.79</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B120" s="7">
         <v>45873</v>
@@ -9402,25 +9403,25 @@
       <c r="N120" s="8">
         <v>0.52300000000000002</v>
       </c>
-      <c r="O120" s="38">
+      <c r="O120" s="9">
         <f>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>9.1000000000000025E-2</v>
       </c>
       <c r="P120" s="36">
         <v>0.51400000000000001</v>
       </c>
-      <c r="Q120" s="42">
+      <c r="Q120" s="40">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>8.2000000000000017E-2</v>
       </c>
-      <c r="R120" s="42">
+      <c r="R120" s="40">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.18999999999999995</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B121" s="7">
         <v>45883</v>
@@ -9472,18 +9473,18 @@
       <c r="P121" s="10">
         <v>0.80400000000000005</v>
       </c>
-      <c r="Q121" s="38">
+      <c r="Q121" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.13400000000000001</v>
       </c>
-      <c r="R121" s="38">
+      <c r="R121" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.28600000000000003</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B122" s="7">
         <v>45873</v>
@@ -9535,18 +9536,18 @@
       <c r="P122" s="10">
         <v>0.871</v>
       </c>
-      <c r="Q122" s="38">
+      <c r="Q122" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.18499999999999994</v>
       </c>
-      <c r="R122" s="38">
+      <c r="R122" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.43900000000000006</v>
       </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B123" s="7">
         <v>45883</v>
@@ -9598,18 +9599,18 @@
       <c r="P123" s="10">
         <v>0.79800000000000004</v>
       </c>
-      <c r="Q123" s="38">
+      <c r="Q123" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.126</v>
       </c>
-      <c r="R123" s="38">
+      <c r="R123" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.34899999999999998</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B124" s="7">
         <v>45883</v>
@@ -9618,9 +9619,9 @@
         <v>96</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E124" s="38" t="str">
+        <v>120</v>
+      </c>
+      <c r="E124" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v>lasiocampidae</v>
       </c>
@@ -9659,18 +9660,18 @@
       <c r="P124" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="Q124" s="38">
+      <c r="Q124" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.6999999999999922E-2</v>
       </c>
-      <c r="R124" s="38">
+      <c r="R124" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.17500000000000004</v>
       </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B125" s="7">
         <v>45873</v>
@@ -9722,18 +9723,18 @@
       <c r="P125" s="10">
         <v>0.70299999999999996</v>
       </c>
-      <c r="Q125" s="38">
+      <c r="Q125" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.9999999999999907E-2</v>
       </c>
-      <c r="R125" s="38">
+      <c r="R125" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B126" s="7">
         <v>45873</v>
@@ -9785,18 +9786,18 @@
       <c r="P126" s="10">
         <v>0.498</v>
       </c>
-      <c r="Q126" s="38">
+      <c r="Q126" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.4999999999999993E-2</v>
       </c>
-      <c r="R126" s="38">
+      <c r="R126" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B127" s="7">
         <v>45883</v>
@@ -9848,18 +9849,18 @@
       <c r="P127" s="10">
         <v>0.69299999999999995</v>
       </c>
-      <c r="Q127" s="38">
+      <c r="Q127" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.2999999999999901E-2</v>
       </c>
-      <c r="R127" s="38">
+      <c r="R127" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>9.6000000000000085E-2</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B128" s="7">
         <v>45873</v>
@@ -9909,18 +9910,18 @@
       <c r="P128" s="10">
         <v>0.72</v>
       </c>
-      <c r="Q128" s="38">
+      <c r="Q128" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>4.1999999999999926E-2</v>
       </c>
-      <c r="R128" s="38">
+      <c r="R128" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.15400000000000003</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B129" s="7">
         <v>45883</v>
@@ -9972,18 +9973,18 @@
       <c r="P129" s="10">
         <v>0.74</v>
       </c>
-      <c r="Q129" s="38">
+      <c r="Q129" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>5.699999999999994E-2</v>
       </c>
-      <c r="R129" s="38">
+      <c r="R129" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.18700000000000006</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B130" s="7">
         <v>45873</v>
@@ -10022,31 +10023,31 @@
         <v>1.0529999999999999</v>
       </c>
       <c r="M130" s="8" t="b">
-        <f t="shared" ref="M130:M161" si="4">L130&lt;I130</f>
+        <f t="shared" ref="M130:M154" si="4">L130&lt;I130</f>
         <v>1</v>
       </c>
       <c r="N130" s="8">
         <v>1.0529999999999999</v>
       </c>
-      <c r="O130" s="38">
+      <c r="O130" s="9">
         <f>Table1[[#This Row],[Dry_Weight_Final]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.37699999999999989</v>
       </c>
       <c r="P130" s="35">
         <v>0.1021</v>
       </c>
-      <c r="Q130" s="41">
+      <c r="Q130">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>-0.57390000000000008</v>
       </c>
-      <c r="R130" s="41">
+      <c r="R130">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>1.7719</v>
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B131" s="7">
         <v>45873</v>
@@ -10096,18 +10097,18 @@
       <c r="P131" s="10">
         <v>0.75700000000000001</v>
       </c>
-      <c r="Q131" s="38">
+      <c r="Q131" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>7.7999999999999958E-2</v>
       </c>
-      <c r="R131" s="38">
+      <c r="R131" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.18000000000000005</v>
       </c>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B132" s="37" t="s">
         <v>102</v>
@@ -10170,7 +10171,7 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B133" s="16">
         <v>45873</v>
@@ -10222,18 +10223,18 @@
       <c r="P133" s="17">
         <v>0.69</v>
       </c>
-      <c r="Q133" s="38">
+      <c r="Q133" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>1.6999999999999904E-2</v>
       </c>
-      <c r="R133" s="38">
+      <c r="R133" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.1180000000000001</v>
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B134" s="16">
         <v>45883</v>
@@ -10287,21 +10288,21 @@
       <c r="P134" s="17">
         <v>0.46899999999999997</v>
       </c>
-      <c r="Q134" s="38">
+      <c r="Q134" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>3.4999999999999976E-2</v>
       </c>
-      <c r="R134" s="38">
+      <c r="R134" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.10200000000000009</v>
       </c>
       <c r="S134" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B135" s="16">
         <v>45873</v>
@@ -10355,21 +10356,21 @@
       <c r="P135" s="17">
         <v>0.79400000000000004</v>
       </c>
-      <c r="Q135" s="38">
+      <c r="Q135" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.10100000000000009</v>
       </c>
-      <c r="R135" s="38">
+      <c r="R135" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.36199999999999988</v>
       </c>
       <c r="S135" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B136" s="16">
         <v>45873</v>
@@ -10380,7 +10381,7 @@
       <c r="D136" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="E136" s="38" t="str">
+      <c r="E136" s="9" t="str">
         <f>Table1[[#This Row],[Family]]&amp;Table1[[#This Row],[Size]]</f>
         <v xml:space="preserve">Limnephilidae </v>
       </c>
@@ -10421,27 +10422,27 @@
       <c r="P136" s="17">
         <v>0.745</v>
       </c>
-      <c r="Q136" s="38">
+      <c r="Q136" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>6.899999999999995E-2</v>
       </c>
-      <c r="R136" s="38">
+      <c r="R136" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.255</v>
       </c>
       <c r="S136" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B137" s="16">
         <v>45883</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D137" s="15" t="s">
         <v>104</v>
@@ -10487,21 +10488,21 @@
       <c r="P137" s="17">
         <v>0.77500000000000002</v>
       </c>
-      <c r="Q137" s="38">
+      <c r="Q137" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>9.3999999999999972E-2</v>
       </c>
-      <c r="R137" s="38">
+      <c r="R137" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.80799999999999994</v>
       </c>
       <c r="S137" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B138" s="16">
         <v>45873</v>
@@ -10551,18 +10552,18 @@
       <c r="P138" s="17">
         <v>0.74299999999999999</v>
       </c>
-      <c r="Q138" s="38">
+      <c r="Q138" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>7.0999999999999952E-2</v>
       </c>
-      <c r="R138" s="38">
+      <c r="R138" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.31199999999999994</v>
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B139" s="16">
         <v>45883</v>
@@ -10613,21 +10614,21 @@
       <c r="P139" s="17">
         <v>0.78600000000000003</v>
       </c>
-      <c r="Q139" s="38">
+      <c r="Q139" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>0.11299999999999999</v>
       </c>
-      <c r="R139" s="38">
+      <c r="R139" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.34600000000000009</v>
       </c>
       <c r="S139" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B140" s="16">
         <v>45873</v>
@@ -10677,18 +10678,18 @@
       <c r="P140" s="17">
         <v>0.75600000000000001</v>
       </c>
-      <c r="Q140" s="38">
+      <c r="Q140" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>4.4000000000000039E-2</v>
       </c>
-      <c r="R140" s="38">
+      <c r="R140" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B141" s="16">
         <v>45873</v>
@@ -10740,18 +10741,18 @@
       <c r="P141" s="17">
         <v>0.73599999999999999</v>
       </c>
-      <c r="Q141" s="38">
+      <c r="Q141" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>4.1000000000000036E-2</v>
       </c>
-      <c r="R141" s="38">
+      <c r="R141" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>6.1000000000000054E-2</v>
       </c>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B142" s="16">
         <v>45873</v>
@@ -10803,18 +10804,18 @@
       <c r="P142" s="17">
         <v>0.70099999999999996</v>
       </c>
-      <c r="Q142" s="38">
+      <c r="Q142" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.4999999999999911E-2</v>
       </c>
-      <c r="R142" s="38">
+      <c r="R142" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B143" s="37">
         <v>45894</v>
@@ -10874,7 +10875,7 @@
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B144" s="16">
         <v>45873</v>
@@ -10926,18 +10927,18 @@
       <c r="P144" s="17">
         <v>0.71599999999999997</v>
       </c>
-      <c r="Q144" s="38">
+      <c r="Q144" s="9">
         <f>Table1[[#This Row],[Lipid Free Weight with envelope]]-Table1[[#This Row],[Envelope+Staple weight]]</f>
         <v>2.9999999999999916E-2</v>
       </c>
-      <c r="R144" s="38">
+      <c r="R144" s="9">
         <f>Table1[[#This Row],[Insect_Weight]]-Table1[[#This Row],[Lipid_Free_Weight]]</f>
         <v>0.14100000000000001</v>
       </c>
     </row>
     <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B145" s="37">
         <v>45894</v>
@@ -11001,7 +11002,7 @@
     </row>
     <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B146" s="37">
         <v>45870</v>
@@ -11065,7 +11066,7 @@
     </row>
     <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B147" s="37">
         <v>45894</v>
@@ -11128,7 +11129,7 @@
     </row>
     <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B148" s="37">
         <v>45907</v>
@@ -11191,7 +11192,7 @@
     </row>
     <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B149" s="37" t="s">
         <v>102</v>
@@ -11251,7 +11252,7 @@
     </row>
     <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B150" s="37">
         <v>45917</v>
@@ -11314,7 +11315,7 @@
     </row>
     <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B151" s="37" t="s">
         <v>102</v>
@@ -11375,7 +11376,7 @@
     </row>
     <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B152" s="37">
         <v>45917</v>
@@ -11497,12 +11498,12 @@
         <v>0.65599999999999992</v>
       </c>
       <c r="S153" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B154" s="29">
         <v>45873</v>

</xml_diff>